<commit_message>
feat: read xlsx file
</commit_message>
<xml_diff>
--- a/assets/files/create_users_template.xlsx
+++ b/assets/files/create_users_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03 Flutter Programming\asco\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BE08497-B076-4115-9E06-3A332D1A5C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E53AD4-D8C9-4ED6-A714-FD869D291D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7BDC27C5-325F-4613-B36F-26AAB32C658E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -51,21 +51,38 @@
     <t>role</t>
   </si>
   <si>
+    <t>cick</t>
+  </si>
+  <si>
+    <t>Muhammad Fajri Rasid</t>
+  </si>
+  <si>
+    <t>ASSISTANT</t>
+  </si>
+  <si>
+    <t>rafmas</t>
+  </si>
+  <si>
+    <t>Rafly Ramadhani Putra</t>
+  </si>
+  <si>
     <t>STUDENT</t>
-  </si>
-  <si>
-    <t>ASSISTANT</t>
-  </si>
-  <si>
-    <t>role:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -93,8 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,7 +427,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08660C1F-C6E5-4FAF-9E73-8FCBFF94433D}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -417,40 +435,61 @@
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>2019</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H3" t="s">
-        <v>6</v>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>2016</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: update some role checker
</commit_message>
<xml_diff>
--- a/assets/files/create_users_template.xlsx
+++ b/assets/files/create_users_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03 Flutter Programming\asco\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E53AD4-D8C9-4ED6-A714-FD869D291D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACF1D89-00ED-4025-90A1-E5487ECCF4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7BDC27C5-325F-4613-B36F-26AAB32C658E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>username</t>
   </si>
@@ -67,6 +67,42 @@
   </si>
   <si>
     <t>STUDENT</t>
+  </si>
+  <si>
+    <t>sony</t>
+  </si>
+  <si>
+    <t>Silverius Sony Lembang</t>
+  </si>
+  <si>
+    <t>H071211001</t>
+  </si>
+  <si>
+    <t>H071211002</t>
+  </si>
+  <si>
+    <t>H071211003</t>
+  </si>
+  <si>
+    <t>H071211004</t>
+  </si>
+  <si>
+    <t>H071211005</t>
+  </si>
+  <si>
+    <t>Wd. Ananda Lesmono</t>
+  </si>
+  <si>
+    <t>Liska Dewi Rombe</t>
+  </si>
+  <si>
+    <t>Dhiya Unnisa</t>
+  </si>
+  <si>
+    <t>Eka Hanni Oktavia</t>
+  </si>
+  <si>
+    <t>Febi Fiantika</t>
   </si>
 </sst>
 </file>
@@ -427,15 +463,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08660C1F-C6E5-4FAF-9E73-8FCBFF94433D}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.21875" customWidth="1"/>
@@ -489,6 +524,108 @@
         <v>2016</v>
       </c>
       <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>2018</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>2021</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>2021</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>2021</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8">
+        <v>2021</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>2021</v>
+      </c>
+      <c r="E9" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: update meeting feature at assistant role
</commit_message>
<xml_diff>
--- a/assets/files/create_users_template.xlsx
+++ b/assets/files/create_users_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03 Flutter Programming\asco\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACF1D89-00ED-4025-90A1-E5487ECCF4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F8CACF-4431-418E-8CA1-6D5A541FD715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7BDC27C5-325F-4613-B36F-26AAB32C658E}"/>
   </bookViews>
@@ -465,7 +465,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08660C1F-C6E5-4FAF-9E73-8FCBFF94433D}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>